<commit_message>
[OPT-3] - Small calculation time fix
</commit_message>
<xml_diff>
--- a/ExcelFormat.xlsx
+++ b/ExcelFormat.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\MS Visual Studio 2019\OPTEL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A28C07F-BE6B-4601-B6C2-9341E4DAFC8F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE4D66A8-0332-486B-992E-4B3B2E3DD689}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="1" activeTab="3" xr2:uid="{3F964C94-F0DC-451B-9B82-1F291A0CA648}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="38">
   <si>
     <t>Name</t>
   </si>
@@ -144,6 +144,9 @@
   </si>
   <si>
     <t>Width, m</t>
+  </si>
+  <si>
+    <t>PredefinedTime</t>
   </si>
 </sst>
 </file>
@@ -643,10 +646,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA776DB7-E681-4B90-8897-81C1B21273F9}">
-  <dimension ref="A1:H1"/>
+  <dimension ref="A1:I1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -659,9 +662,10 @@
     <col min="6" max="6" width="24.21875" customWidth="1"/>
     <col min="7" max="7" width="21.5546875" customWidth="1"/>
     <col min="8" max="8" width="22.21875" customWidth="1"/>
+    <col min="9" max="9" width="16.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="31.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" ht="31.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
         <v>6</v>
       </c>
@@ -685,6 +689,9 @@
       </c>
       <c r="H1" s="3" t="s">
         <v>31</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[OPT-2][OPT-15] - Setted new fields to databases + target functions calculators fix + excel parsers fix + template fix
</commit_message>
<xml_diff>
--- a/ExcelFormat.xlsx
+++ b/ExcelFormat.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24026"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\source\repos\optel3.desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\MS Visual Studio 2019\OPTEL\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57CF0CF2-0816-4AEF-8DB7-282096EE1583}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570" firstSheet="1" activeTab="8"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="2" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="FilmTypes" sheetId="9" r:id="rId1"/>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="44">
   <si>
     <t>Name</t>
   </si>
@@ -58,9 +59,6 @@
     <t>Production speed, m/h</t>
   </si>
   <si>
-    <t>Material cost, EUR/kg</t>
-  </si>
-  <si>
     <t>Film type article</t>
   </si>
   <si>
@@ -73,15 +71,6 @@
     <t>Quantity in running meter, m</t>
   </si>
   <si>
-    <t>Nozzle, mk</t>
-  </si>
-  <si>
-    <t>Calibration, mk</t>
-  </si>
-  <si>
-    <t>Cooling lip, mk</t>
-  </si>
-  <si>
     <t>Nozzle to change, mk</t>
   </si>
   <si>
@@ -91,18 +80,9 @@
     <t>Cooling lip to change, mk</t>
   </si>
   <si>
-    <t>Price overdue, EUR/h</t>
-  </si>
-  <si>
     <t>Max production speed, m/min</t>
   </si>
   <si>
-    <t>Width min, m</t>
-  </si>
-  <si>
-    <t>Width max, m</t>
-  </si>
-  <si>
     <t>Thickness min, µm</t>
   </si>
   <si>
@@ -124,34 +104,73 @@
     <t>Length max, m</t>
   </si>
   <si>
-    <t>Thickness change time, s</t>
-  </si>
-  <si>
     <t>Customer name</t>
   </si>
   <si>
-    <t>Width change time, s</t>
-  </si>
-  <si>
-    <t>Article film type to change</t>
-  </si>
-  <si>
-    <t>Article film type from change</t>
-  </si>
-  <si>
-    <t>Predefined time, min</t>
-  </si>
-  <si>
-    <t>Width, m</t>
-  </si>
-  <si>
-    <t>PredefinedTime, h</t>
+    <t>Nozzle, DN</t>
+  </si>
+  <si>
+    <t>Calibration, DN</t>
+  </si>
+  <si>
+    <t>Cooling lip, DN</t>
+  </si>
+  <si>
+    <t>Number</t>
+  </si>
+  <si>
+    <t>Width</t>
+  </si>
+  <si>
+    <t>FinishedGoods, kg</t>
+  </si>
+  <si>
+    <t>Waste, kg</t>
+  </si>
+  <si>
+    <t>RollsCount</t>
+  </si>
+  <si>
+    <t>PredefinedTime, min</t>
+  </si>
+  <si>
+    <t>Price overdue, €/h</t>
+  </si>
+  <si>
+    <t>Material cost, €/kg</t>
+  </si>
+  <si>
+    <t>Width min, mm</t>
+  </si>
+  <si>
+    <t>Width max, mm</t>
+  </si>
+  <si>
+    <t>Thickness change time, min</t>
+  </si>
+  <si>
+    <t>Thickness change consumption, kg/h</t>
+  </si>
+  <si>
+    <t>Width change time, min</t>
+  </si>
+  <si>
+    <t>Width change consumption, kg/h</t>
+  </si>
+  <si>
+    <t>Name recipe from change</t>
+  </si>
+  <si>
+    <t>Name recipe to change</t>
+  </si>
+  <si>
+    <t>Consumption, kg/h</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -537,21 +556,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.5703125" customWidth="1"/>
+    <col min="1" max="1" width="10.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="23.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" ht="23.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -561,53 +580,53 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="21.140625" customWidth="1"/>
-    <col min="3" max="3" width="22.140625" customWidth="1"/>
+    <col min="2" max="2" width="21.109375" customWidth="1"/>
+    <col min="3" max="3" width="22.109375" customWidth="1"/>
     <col min="4" max="4" width="23" customWidth="1"/>
-    <col min="5" max="5" width="23.140625" customWidth="1"/>
-    <col min="6" max="6" width="16.7109375" customWidth="1"/>
-    <col min="7" max="7" width="16.5703125" customWidth="1"/>
-    <col min="8" max="8" width="15.5703125" customWidth="1"/>
-    <col min="9" max="9" width="17.28515625" customWidth="1"/>
-    <col min="10" max="10" width="17.140625" customWidth="1"/>
+    <col min="5" max="5" width="23.109375" customWidth="1"/>
+    <col min="6" max="6" width="16.6640625" customWidth="1"/>
+    <col min="7" max="7" width="16.5546875" customWidth="1"/>
+    <col min="8" max="8" width="15.5546875" customWidth="1"/>
+    <col min="9" max="9" width="17.33203125" customWidth="1"/>
+    <col min="10" max="10" width="17.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="28.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" ht="28.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>7</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>8</v>
+        <v>34</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>13</v>
+        <v>24</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>15</v>
+        <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="1"/>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
@@ -623,19 +642,25 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:B1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.85546875" customWidth="1"/>
+    <col min="1" max="1" width="17.88671875" customWidth="1"/>
+    <col min="2" max="2" width="16.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -644,53 +669,61 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <dimension ref="A1:K1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.7109375" customWidth="1"/>
-    <col min="2" max="2" width="14.140625" customWidth="1"/>
-    <col min="3" max="3" width="29.5703125" customWidth="1"/>
-    <col min="4" max="4" width="18.42578125" customWidth="1"/>
-    <col min="5" max="5" width="21.7109375" customWidth="1"/>
-    <col min="6" max="6" width="24.28515625" customWidth="1"/>
-    <col min="7" max="7" width="21.5703125" customWidth="1"/>
-    <col min="8" max="8" width="22.28515625" customWidth="1"/>
-    <col min="9" max="9" width="16.7109375" customWidth="1"/>
+    <col min="1" max="1" width="14.6640625" customWidth="1"/>
+    <col min="2" max="2" width="14.109375" customWidth="1"/>
+    <col min="3" max="3" width="29.5546875" customWidth="1"/>
+    <col min="4" max="4" width="18.44140625" customWidth="1"/>
+    <col min="5" max="5" width="21.6640625" customWidth="1"/>
+    <col min="6" max="6" width="24.33203125" customWidth="1"/>
+    <col min="7" max="7" width="21.5546875" customWidth="1"/>
+    <col min="8" max="8" width="22.33203125" customWidth="1"/>
+    <col min="9" max="9" width="16.6640625" customWidth="1"/>
+    <col min="10" max="10" width="18.109375" customWidth="1"/>
+    <col min="11" max="11" width="14.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" ht="31.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="3" t="s">
-        <v>36</v>
+      <c r="B1" s="4" t="s">
+        <v>28</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D1" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="H1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>31</v>
-      </c>
       <c r="I1" s="3" t="s">
-        <v>37</v>
+        <v>10</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -699,33 +732,34 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+  <dimension ref="A1:P1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="N9" sqref="N9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.140625" customWidth="1"/>
-    <col min="2" max="2" width="12.28515625" customWidth="1"/>
-    <col min="3" max="3" width="21.7109375" customWidth="1"/>
-    <col min="4" max="4" width="28.85546875" customWidth="1"/>
-    <col min="5" max="5" width="15.140625" customWidth="1"/>
+    <col min="1" max="1" width="15.109375" customWidth="1"/>
+    <col min="2" max="2" width="12.33203125" customWidth="1"/>
+    <col min="3" max="3" width="21.6640625" customWidth="1"/>
+    <col min="4" max="4" width="28.88671875" customWidth="1"/>
+    <col min="5" max="5" width="15.109375" customWidth="1"/>
     <col min="6" max="6" width="17" customWidth="1"/>
-    <col min="7" max="7" width="20.42578125" customWidth="1"/>
-    <col min="8" max="8" width="21.85546875" customWidth="1"/>
-    <col min="9" max="9" width="19.140625" customWidth="1"/>
+    <col min="7" max="7" width="20.44140625" customWidth="1"/>
+    <col min="8" max="8" width="21.88671875" customWidth="1"/>
+    <col min="9" max="9" width="19.109375" customWidth="1"/>
     <col min="10" max="10" width="19" customWidth="1"/>
-    <col min="11" max="11" width="18.7109375" customWidth="1"/>
+    <col min="11" max="11" width="18.6640625" customWidth="1"/>
     <col min="12" max="12" width="17" customWidth="1"/>
-    <col min="13" max="13" width="22.42578125" customWidth="1"/>
-    <col min="14" max="14" width="25" customWidth="1"/>
-    <col min="15" max="15" width="27" customWidth="1"/>
+    <col min="13" max="13" width="22.44140625" customWidth="1"/>
+    <col min="14" max="14" width="22.88671875" customWidth="1"/>
+    <col min="15" max="15" width="24.33203125" customWidth="1"/>
+    <col min="16" max="16" width="20.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="29.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" ht="29.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -736,37 +770,43 @@
         <v>3</v>
       </c>
       <c r="D1" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="J1" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="K1" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="L1" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="G1" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="K1" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="L1" s="3" t="s">
-        <v>29</v>
-      </c>
       <c r="M1" s="3" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="N1" s="3" t="s">
-        <v>30</v>
+        <v>38</v>
+      </c>
+      <c r="O1" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="P1" s="3" t="s">
+        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -775,33 +815,37 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+  <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection sqref="A1:E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="18.28515625" customWidth="1"/>
-    <col min="2" max="2" width="28.85546875" customWidth="1"/>
-    <col min="3" max="3" width="26.42578125" customWidth="1"/>
-    <col min="4" max="4" width="27.42578125" customWidth="1"/>
+    <col min="1" max="1" width="18.33203125" customWidth="1"/>
+    <col min="2" max="2" width="28.88671875" customWidth="1"/>
+    <col min="3" max="3" width="26.44140625" customWidth="1"/>
+    <col min="4" max="4" width="27.44140625" customWidth="1"/>
+    <col min="5" max="5" width="22.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="28.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" ht="28.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>34</v>
+        <v>41</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>33</v>
+        <v>42</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>5</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>43</v>
       </c>
     </row>
   </sheetData>
@@ -811,29 +855,33 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+  <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.85546875" customWidth="1"/>
-    <col min="2" max="2" width="24.28515625" customWidth="1"/>
-    <col min="3" max="3" width="29.28515625" customWidth="1"/>
+    <col min="1" max="1" width="15.88671875" customWidth="1"/>
+    <col min="2" max="2" width="24.33203125" customWidth="1"/>
+    <col min="3" max="3" width="29.33203125" customWidth="1"/>
+    <col min="4" max="4" width="19.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="36.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" ht="36.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>5</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>43</v>
       </c>
     </row>
   </sheetData>
@@ -842,29 +890,33 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+  <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.42578125" customWidth="1"/>
-    <col min="2" max="2" width="25.7109375" customWidth="1"/>
+    <col min="1" max="1" width="19.44140625" customWidth="1"/>
+    <col min="2" max="2" width="25.6640625" customWidth="1"/>
     <col min="3" max="3" width="31" customWidth="1"/>
+    <col min="4" max="4" width="21.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="31.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" ht="31.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>5</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>43</v>
       </c>
     </row>
   </sheetData>
@@ -873,29 +925,33 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+  <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="18.85546875" customWidth="1"/>
-    <col min="2" max="2" width="28.28515625" customWidth="1"/>
-    <col min="3" max="3" width="30.7109375" customWidth="1"/>
+    <col min="1" max="1" width="18.88671875" customWidth="1"/>
+    <col min="2" max="2" width="28.33203125" customWidth="1"/>
+    <col min="3" max="3" width="30.6640625" customWidth="1"/>
+    <col min="4" max="4" width="21.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="34.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" ht="34.950000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>5</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>